<commit_message>
Update matrix to point SIAC steps to AUTH-PATIENT-18
</commit_message>
<xml_diff>
--- a/public/downloads/onc_program_matrix_1_6_2.xlsx
+++ b/public/downloads/onc_program_matrix_1_6_2.xlsx
@@ -2450,7 +2450,7 @@
       <c r="AZ7" s="1" t="str">
         <v/>
       </c>
-      <c r="BA7" s="133" t="str">
+      <c r="BA7" s="1" t="str">
         <v/>
       </c>
       <c r="BB7" s="155" t="str">
@@ -5238,7 +5238,7 @@
       <c r="AZ24" s="1" t="str">
         <v/>
       </c>
-      <c r="BA24" s="1" t="str">
+      <c r="BA24" s="133" t="str">
         <v/>
       </c>
       <c r="BB24" s="155" t="str">
@@ -11880,7 +11880,7 @@
         <v>yes</v>
       </c>
       <c r="H14" s="160" t="str">
-        <v>SPB-OSLS-01, SPB-OSLS-02, SPB-OSLS-03, SPB-OSLS-04, SPB-OSLS-05, SPB-OSLS-06, SPB-OSLS-07, SPB-OSLS-08, SPB-OSLS-09, EHB-OELS-01, EHB-OELS-02, EHB-OELS-03, EHB-OELS-04, EHB-OELS-05, EHB-OELS-06, EHB-OELS-07, EHB-OELS-08, EHB-OELS-09, EHB-OELS-10, EHB-OELS-11, SIAC-01, SIAC-02, SIAC-03, SIAC-04</v>
+        <v>SPB-OSLS-01, SPB-OSLS-02, SPB-OSLS-03, SPB-OSLS-04, SPB-OSLS-05, SPB-OSLS-06, SPB-OSLS-07, SPB-OSLS-08, SPB-OSLS-09, EHB-OELS-01, EHB-OELS-02, EHB-OELS-03, EHB-OELS-04, EHB-OELS-05, EHB-OELS-06, EHB-OELS-07, EHB-OELS-08, EHB-OELS-09, EHB-OELS-10, EHB-OELS-11</v>
       </c>
       <c r="I14" s="160" t="str">
         <v xml:space="preserve">Complete demonstration of these capabilities are accomplished
@@ -12587,7 +12587,7 @@
         <v>yes</v>
       </c>
       <c r="H31" s="160" t="str">
-        <v>RPA-OSRLS-02, RPA-OSRLS-03, RPA-OSRLS-04, RPA-OSRLS-05, RPA-OSRLS-06, RPA-OSRLS-07, RPA-OSRLS-08, RPA-OSRLS-09, RPA-OSRLS-10, RPA-OSRLS-11, AVR-01, AVR-02, AVR-03, AVR-04, AVR-05, AVR-06, AVR-07, AVR-08, AVR-09, AVR-10, AVR-11, AVR-12, AVR-13, AVR-14</v>
+        <v>RPA-OSRLS-02, RPA-OSRLS-03, RPA-OSRLS-04, RPA-OSRLS-05, RPA-OSRLS-06, RPA-OSRLS-07, RPA-OSRLS-08, RPA-OSRLS-09, RPA-OSRLS-10, RPA-OSRLS-11, AVR-01, AVR-02, AVR-03, AVR-04, AVR-05, AVR-06, AVR-07, AVR-08, AVR-09, AVR-10, AVR-11, AVR-12, AVR-13, AVR-14, SIAC-01, SIAC-02, SIAC-03, SIAC-04</v>
       </c>
       <c r="I31" s="160" t="str">
         <v xml:space="preserve">Inferno verifies that the user has the ability to explicitly authorize
@@ -24241,7 +24241,7 @@
         <v>http://www.hl7.org/fhir/smart-app-launch/</v>
       </c>
       <c r="G433" s="160" t="str">
-        <v>AUTH-PATIENT-1</v>
+        <v>AUTH-PATIENT-18</v>
       </c>
     </row>
     <row r="434" spans="1:7" s="159" customFormat="1" ht="30" customHeight="1">
@@ -24265,7 +24265,7 @@
         <v>http://www.hl7.org/fhir/smart-app-launch/</v>
       </c>
       <c r="G434" s="160" t="str">
-        <v>AUTH-PATIENT-1</v>
+        <v>AUTH-PATIENT-18</v>
       </c>
     </row>
     <row r="435" spans="1:7" s="159" customFormat="1" ht="30" customHeight="1">
@@ -24289,7 +24289,7 @@
         <v>https://tools.ietf.org/html/rfc6749</v>
       </c>
       <c r="G435" s="160" t="str">
-        <v>AUTH-PATIENT-1</v>
+        <v>AUTH-PATIENT-18</v>
       </c>
     </row>
     <row r="436" spans="1:7" s="159" customFormat="1" ht="30" customHeight="1">
@@ -24313,7 +24313,7 @@
         <v>https://tools.ietf.org/html/rfc6749</v>
       </c>
       <c r="G436" s="160" t="str">
-        <v>AUTH-PATIENT-1</v>
+        <v>AUTH-PATIENT-18</v>
       </c>
     </row>
     <row r="437" spans="2:2" customFormat="false">

</xml_diff>

<commit_message>
Fix attestion for token refresh timeout.
</commit_message>
<xml_diff>
--- a/public/downloads/onc_program_matrix_1_6_2.xlsx
+++ b/public/downloads/onc_program_matrix_1_6_2.xlsx
@@ -24424,10 +24424,10 @@
         <v>ATT-05</v>
       </c>
       <c r="D442" s="160" t="str">
-        <v>Health IT Module attested that refresh tokens had three month timeout period.</v>
+        <v>Health IT Module attested that refresh tokens are valid for a period of no shorter than three months.</v>
       </c>
       <c r="E442" s="160" t="str">
-        <v>Health IT Module attested that refresh tokens had three month timeout period.</v>
+        <v>Health IT Module attested that refresh tokens are valid for a period of no shorter than three months.</v>
       </c>
       <c r="F442" s="160" t="str">
         <v>https://www.federalregister.gov/documents/2020/05/01/2020-07419/21st-century-cures-act-interoperability-information-blocking-and-the-onc-health-it-certification</v>

</xml_diff>